<commit_message>
comparison with BDS and TO
on their representative images
</commit_message>
<xml_diff>
--- a/Result/AIO.xlsx
+++ b/Result/AIO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>1_1 vs 3_1</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>ours2 vs offset statistics</t>
+  </si>
+  <si>
+    <t>ours vs texture optimization</t>
+  </si>
+  <si>
+    <t>ours vs bds</t>
+  </si>
+  <si>
+    <t>10/3(43)</t>
+  </si>
+  <si>
+    <t>10/4(43)</t>
   </si>
 </sst>
 </file>
@@ -347,12 +359,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="65764864"/>
-        <c:axId val="95167616"/>
+        <c:axId val="538727424"/>
+        <c:axId val="98815936"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="65764864"/>
+        <c:axId val="538727424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -361,7 +373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95167616"/>
+        <c:crossAx val="98815936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -369,7 +381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95167616"/>
+        <c:axId val="98815936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,7 +392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65764864"/>
+        <c:crossAx val="538727424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -618,12 +630,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="65762816"/>
-        <c:axId val="95169344"/>
+        <c:axId val="555504128"/>
+        <c:axId val="98818240"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="65762816"/>
+        <c:axId val="555504128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95169344"/>
+        <c:crossAx val="98818240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -640,7 +652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95169344"/>
+        <c:axId val="98818240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,7 +663,242 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65762816"/>
+        <c:crossAx val="555504128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>worse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$55:$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ours vs texture optimization</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ours vs bds</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$56:$C$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.9800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Not sure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$55:$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ours vs texture optimization</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ours vs bds</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$57:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.6976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>better</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$55:$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ours vs texture optimization</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ours vs bds</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$58:$C$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.2326</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="53681152"/>
+        <c:axId val="77161600"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="53681152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77161600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="77161600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53681152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -730,6 +977,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1025,15 +1302,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
     <col min="2" max="2" width="22.81640625" customWidth="1"/>
     <col min="3" max="3" width="24.08984375" customWidth="1"/>
     <col min="4" max="4" width="23.26953125" customWidth="1"/>
@@ -1220,6 +1497,63 @@
       </c>
       <c r="E32">
         <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56">
+        <v>6.9800000000000001E-2</v>
+      </c>
+      <c r="C56">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57">
+        <v>0.6976</v>
+      </c>
+      <c r="C57">
+        <v>0.6744</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58">
+        <v>0.2326</v>
+      </c>
+      <c r="C58">
+        <v>0.2326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
synthesis and user study finished.
</commit_message>
<xml_diff>
--- a/Result/AIO.xlsx
+++ b/Result/AIO.xlsx
@@ -359,12 +359,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="538727424"/>
-        <c:axId val="98815936"/>
+        <c:axId val="548758528"/>
+        <c:axId val="107794368"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="538727424"/>
+        <c:axId val="548758528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98815936"/>
+        <c:crossAx val="107794368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -381,7 +381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98815936"/>
+        <c:axId val="107794368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,7 +392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="538727424"/>
+        <c:crossAx val="548758528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -630,12 +630,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="555504128"/>
-        <c:axId val="98818240"/>
+        <c:axId val="565535232"/>
+        <c:axId val="107796672"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="555504128"/>
+        <c:axId val="565535232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98818240"/>
+        <c:crossAx val="107796672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -652,7 +652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98818240"/>
+        <c:axId val="107796672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555504128"/>
+        <c:crossAx val="565535232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -692,10 +692,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
+      <c14:style val="135"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="3"/>
+      <c:style val="35"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -865,12 +865,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="53681152"/>
-        <c:axId val="77161600"/>
+        <c:axId val="565536256"/>
+        <c:axId val="565936704"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53681152"/>
+        <c:axId val="565536256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -879,7 +879,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77161600"/>
+        <c:crossAx val="565936704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -887,7 +887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77161600"/>
+        <c:axId val="565936704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +898,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53681152"/>
+        <c:crossAx val="565536256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1304,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
commit after TOG submission
</commit_message>
<xml_diff>
--- a/Result/AIO.xlsx
+++ b/Result/AIO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="238" yWindow="109" windowWidth="14807" windowHeight="8014"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>1_1 vs 3_1</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>No preference</t>
+  </si>
+  <si>
+    <t>ours2 vs [He and Sun 2012]</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
                   <c:v>ours1 vs [He and Sun 2012]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ours1 vs [He and Sun 2012]</c:v>
+                  <c:v>ours2 vs [He and Sun 2012]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -271,7 +274,7 @@
                   <c:v>ours1 vs [He and Sun 2012]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ours1 vs [He and Sun 2012]</c:v>
+                  <c:v>ours2 vs [He and Sun 2012]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -328,7 +331,7 @@
                   <c:v>ours1 vs [He and Sun 2012]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ours1 vs [He and Sun 2012]</c:v>
+                  <c:v>ours2 vs [He and Sun 2012]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -365,12 +368,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="541915648"/>
-        <c:axId val="80713920"/>
+        <c:axId val="536088064"/>
+        <c:axId val="116495424"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="541915648"/>
+        <c:axId val="536088064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -379,7 +382,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80713920"/>
+        <c:crossAx val="116495424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -387,7 +390,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80713920"/>
+        <c:axId val="116495424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +401,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541915648"/>
+        <c:crossAx val="536088064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -600,12 +603,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="541916672"/>
-        <c:axId val="558326336"/>
+        <c:axId val="539673088"/>
+        <c:axId val="116497728"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="541916672"/>
+        <c:axId val="539673088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,7 +617,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="558326336"/>
+        <c:crossAx val="116497728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -622,7 +625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="558326336"/>
+        <c:axId val="116497728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,7 +636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541916672"/>
+        <c:crossAx val="539673088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -720,7 +723,7 @@
                   <c:v>ours1 vs [He and Sun 2012]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ours1 vs [He and Sun 2012]</c:v>
+                  <c:v>ours2 vs [He and Sun 2012]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -777,7 +780,7 @@
                   <c:v>ours1 vs [He and Sun 2012]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ours1 vs [He and Sun 2012]</c:v>
+                  <c:v>ours2 vs [He and Sun 2012]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -834,7 +837,7 @@
                   <c:v>ours1 vs [He and Sun 2012]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>ours1 vs [He and Sun 2012]</c:v>
+                  <c:v>ours2 vs [He and Sun 2012]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -871,12 +874,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="516400128"/>
-        <c:axId val="516528896"/>
+        <c:axId val="539673600"/>
+        <c:axId val="539559616"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="516400128"/>
+        <c:axId val="539673600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="516528896"/>
+        <c:crossAx val="539559616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -893,7 +896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="516528896"/>
+        <c:axId val="539559616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,7 +907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="516400128"/>
+        <c:crossAx val="539673600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1310,11 +1313,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.81640625" customWidth="1"/>
     <col min="2" max="2" width="22.81640625" customWidth="1"/>
@@ -1386,7 +1389,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1451,7 +1454,7 @@
         <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1574,7 +1577,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1586,7 +1589,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Last commit under windows
</commit_message>
<xml_diff>
--- a/Result/AIO.xlsx
+++ b/Result/AIO.xlsx
@@ -144,6 +144,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCD7371"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -159,31 +164,17 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="135"/>
+      <c14:style val="110"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="35"/>
+      <c:style val="10"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:bar3DChart>
+      <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
@@ -201,6 +192,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -258,6 +259,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -315,6 +326,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="CD7371"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -367,13 +388,12 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="536088064"/>
-        <c:axId val="116495424"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
+        <c:overlap val="100"/>
+        <c:axId val="543178240"/>
+        <c:axId val="518755392"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="536088064"/>
+        <c:axId val="543178240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -382,7 +402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116495424"/>
+        <c:crossAx val="518755392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -390,7 +410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116495424"/>
+        <c:axId val="518755392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -401,7 +421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536088064"/>
+        <c:crossAx val="543178240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -430,31 +450,17 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="135"/>
+      <c14:style val="110"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="35"/>
+      <c:style val="10"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:bar3DChart>
+      <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
@@ -472,6 +478,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -517,6 +533,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -562,6 +588,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="CD7371"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -602,13 +638,12 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="539673088"/>
-        <c:axId val="116497728"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
+        <c:overlap val="100"/>
+        <c:axId val="560718336"/>
+        <c:axId val="518757696"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="539673088"/>
+        <c:axId val="560718336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +652,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116497728"/>
+        <c:crossAx val="518757696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -625,7 +660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116497728"/>
+        <c:axId val="518757696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +671,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539673088"/>
+        <c:crossAx val="560718336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -665,31 +700,17 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
+      <c14:style val="110"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="3"/>
+      <c:style val="10"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:bar3DChart>
+      <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
@@ -707,6 +728,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -764,6 +795,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -821,6 +862,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="CD7371"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -873,13 +924,12 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="539673600"/>
-        <c:axId val="539559616"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
+        <c:overlap val="100"/>
+        <c:axId val="560718848"/>
+        <c:axId val="560596672"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="539673600"/>
+        <c:axId val="560718848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539559616"/>
+        <c:crossAx val="560596672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -896,7 +946,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539559616"/>
+        <c:axId val="560596672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539673600"/>
+        <c:crossAx val="560718848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1313,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>

</xml_diff>